<commit_message>
arrumei o arquivo sujo
</commit_message>
<xml_diff>
--- a/Projeto 1/New HIV infections_Number of new HIV infections_Population_2017.xlsx
+++ b/Projeto 1/New HIV infections_Number of new HIV infections_Population_2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b26f2b439bb4d4e/Faculdade/Insper/2ºSemestre/Ciência dos dados/CD/Projeto 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Faculdade\Insper\2ºSemestre\Ciência dos dados\CD\Projeto 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7816239-BC35-4795-932F-B324707F35F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{D7816239-BC35-4795-932F-B324707F35F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{FE36FA03-FB00-45CC-B1AF-B6FCA5C00E22}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Number of new HIV infectio" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Selected Regions</t>
   </si>
@@ -31,127 +31,67 @@
     <t>Angola</t>
   </si>
   <si>
-    <t>29000 [22000 - 36000]</t>
-  </si>
-  <si>
     <t>Botswana</t>
   </si>
   <si>
-    <t>9000 [7600 - 10000]</t>
-  </si>
-  <si>
     <t>Comoros</t>
   </si>
   <si>
-    <t>0 [ - 10]</t>
-  </si>
-  <si>
     <t>Eritrea</t>
   </si>
   <si>
-    <t>610 [330 - 1100]</t>
-  </si>
-  <si>
     <t>Ethiopia</t>
   </si>
   <si>
-    <t>23000 [14000 - 42000]</t>
-  </si>
-  <si>
     <t>Kenya</t>
   </si>
   <si>
-    <t>48000 [28000 - 82000]</t>
-  </si>
-  <si>
     <t>Lesotho</t>
   </si>
   <si>
-    <t>14000 [13000 - 16000]</t>
-  </si>
-  <si>
     <t>Madagascar</t>
   </si>
   <si>
-    <t>5200 [3500 - 8800]</t>
-  </si>
-  <si>
     <t>Mozambique</t>
   </si>
   <si>
-    <t>150000 [91000 - 230000]</t>
-  </si>
-  <si>
     <t>Mauritius</t>
   </si>
   <si>
-    <t>900 [550 - 1300]</t>
-  </si>
-  <si>
     <t>Malawi</t>
   </si>
   <si>
-    <t>40000 [36000 - 46000]</t>
-  </si>
-  <si>
     <t>Namibia</t>
   </si>
   <si>
-    <t>6600 [5500 - 7400]</t>
-  </si>
-  <si>
     <t>Rwanda</t>
   </si>
   <si>
-    <t>4000 [2900 - 5300]</t>
-  </si>
-  <si>
     <t>South Sudan</t>
   </si>
   <si>
-    <t>18000 [12000 - 25000]</t>
-  </si>
-  <si>
     <t>Eswatini</t>
   </si>
   <si>
-    <t>8400 [7500 - 9500]</t>
-  </si>
-  <si>
     <t>United Republic of Tanzania</t>
   </si>
   <si>
-    <t>76000 [65000 - 85000]</t>
-  </si>
-  <si>
     <t>Uganda</t>
   </si>
   <si>
-    <t>58000 [49000 - 73000]</t>
-  </si>
-  <si>
     <t>South Africa</t>
   </si>
   <si>
-    <t>260000 [240000 - 290000]</t>
-  </si>
-  <si>
     <t>Zambia</t>
   </si>
   <si>
-    <t>49000 [35000 - 69000]</t>
-  </si>
-  <si>
     <t>Zimbabwe</t>
-  </si>
-  <si>
-    <t>41000 [30000 - 55000]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -993,10 +933,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1016,160 +958,160 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2">
+        <v>29000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>9000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>610</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>23000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>48000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>14000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>5200</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>150000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>900</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>40000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>6600</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>4000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>18000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>8400</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>76000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>58000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>260000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>49000</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>41000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>